<commit_message>
modifying a few things
</commit_message>
<xml_diff>
--- a/util/csv_jpvoca양식.xlsx
+++ b/util/csv_jpvoca양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unistackr0-my.sharepoint.com/personal/psw1023_unist_ac_kr/Documents/coding practice file/quiz web proj/util/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{85A57A60-CB06-4948-BF95-E0658BA8C546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AA76DE2-E4CF-4A82-98E4-0E35B85D4961}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{85A57A60-CB06-4948-BF95-E0658BA8C546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{189F50AC-7409-4A6C-AB0D-F56D11E9E2E7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{442EF2C4-8967-4167-B468-7A6FE47A263D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,6 +59,358 @@
   </si>
   <si>
     <t>등록일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>じょうずだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>すきだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ふべんだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>とおい</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>きれいだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しずかだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しんせつだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>べんりだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ほんとうだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>にぎやかだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>きらだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>へただ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ハンサムだ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あう</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>いく</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>はなす</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>まつ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しぬ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あそぶ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>よむ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>わかる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>つくる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>のる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>みる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>たべる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>する</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>くる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>はいる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>しる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>かえる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帰る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>見る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>読む</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>食べる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>のむ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飲む</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>うたう</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>おくる</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>べんきょうする</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>かく</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>きく</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>あるく</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歌う</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>勉強する</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書く</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聞く</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>歩く</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>형용사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불편하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멀다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깨끗하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조용하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>친절하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편리하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번화하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>싫어하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 못하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘생기다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만나다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이야기하다", "말하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기다리다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>놀다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>읽다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만들다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>먹다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>들어오다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌아가다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마시다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보내다", "전송하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쓰다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공부하다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>듣다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>걷다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -66,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +440,13 @@
       <name val="Yu Gothic"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,11 +471,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,18 +799,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B9EDB5-9AB6-4DED-AA05-CC585E342F87}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="6" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,71 +830,673 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18.75">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18.75">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.75">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18.75">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18.75">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18.75">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18.75">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18.75">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18.75">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18.75">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18.75">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="18.75">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18.75">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37">
+        <v>230222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18.75">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38">
+        <v>230222</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>